<commit_message>
results of the experiments
</commit_message>
<xml_diff>
--- a/experiments-results.xlsx
+++ b/experiments-results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oussa\Desktop\Canada\Papers\sosym-ai-2021\writing\Experiments-MODELS2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oussa\Desktop\Canada\Papers\sosym-ai-2021\writing\Experiments-MODELS2021\github-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DB0E78-3ECF-4B0E-847D-723DE5BC0A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE8F0C6-6BD9-44B2-9B4D-A2740432A249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7280,7 +7280,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>